<commit_message>
Combining experimental datasets for linear regressions
</commit_message>
<xml_diff>
--- a/experimental_data/GEC_aging/Schnegg1986.xlsx
+++ b/experimental_data/GEC_aging/Schnegg1986.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="98">
   <si>
     <t>Schnegg1986 – Quantitative Liver Function in the Elderly Assessed by GEC</t>
   </si>
@@ -200,7 +200,7 @@
     <t>Table 3</t>
   </si>
   <si>
-    <t> n GEC</t>
+    <t>n GEC</t>
   </si>
   <si>
     <t>mean age GEC [years]</t>
@@ -230,7 +230,7 @@
     <t>Caffeine saliva clearance [ml/min/kg] SD</t>
   </si>
   <si>
-    <t> n AP</t>
+    <t>n AP</t>
   </si>
   <si>
     <t>mean age AP [years]</t>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t>Aminopyrine breath test [% dose kg mmol/Co2]</t>
+  </si>
+  <si>
+    <t>GECmgkg</t>
   </si>
 </sst>
 </file>
@@ -315,7 +318,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -360,11 +363,18 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -579,10 +589,28 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1"/>
+              <a:t>Figure 1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -604,7 +632,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="000000"/>
+              <a:srgbClr val="99ccff"/>
             </a:solidFill>
             <a:ln w="28800">
               <a:noFill/>
@@ -1196,11 +1224,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="37693700"/>
-        <c:axId val="57594254"/>
+        <c:axId val="27165828"/>
+        <c:axId val="27374079"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="37693700"/>
+        <c:axId val="27165828"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1216,7 +1244,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
+                  <a:rPr b="1" sz="900"/>
                   <a:t>age [years]</a:t>
                 </a:r>
               </a:p>
@@ -1234,11 +1262,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="57594254"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="27374079"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57594254"/>
+        <c:axId val="27374079"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -1255,7 +1283,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
+                  <a:rPr b="1" sz="900"/>
                   <a:t>Galactose elimination capacity [mg/min/kg]</a:t>
                 </a:r>
               </a:p>
@@ -1273,7 +1301,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="37693700"/>
+        <c:crossAx val="27165828"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="2"/>
       </c:valAx>
@@ -1299,10 +1327,28 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1"/>
+              <a:t>Caf</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1324,14 +1370,14 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="000000"/>
+              <a:srgbClr val="99ccff"/>
             </a:solidFill>
             <a:ln w="28800">
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="3"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1574,11 +1620,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="4918795"/>
-        <c:axId val="46604859"/>
+        <c:axId val="25719660"/>
+        <c:axId val="93185855"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="4918795"/>
+        <c:axId val="25719660"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="90"/>
@@ -1596,7 +1642,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
+                  <a:rPr b="1" sz="900"/>
                   <a:t>age [years]</a:t>
                 </a:r>
               </a:p>
@@ -1614,12 +1660,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="46604859"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="93185855"/>
+        <c:crossesAt val="0"/>
         <c:majorUnit val="20"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46604859"/>
+        <c:axId val="93185855"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.5"/>
@@ -1637,7 +1683,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
+                  <a:rPr b="1" sz="900"/>
                   <a:t>Caffeine clearance [ml/min/kg]</a:t>
                 </a:r>
               </a:p>
@@ -1655,7 +1701,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="4918795"/>
+        <c:crossAx val="25719660"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="1"/>
       </c:valAx>
@@ -1681,10 +1727,28 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1"/>
+              <a:t>AP</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1706,14 +1770,14 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="000000"/>
+              <a:srgbClr val="99ccff"/>
             </a:solidFill>
             <a:ln w="28800">
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="3"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1992,11 +2056,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="16995230"/>
-        <c:axId val="18718344"/>
+        <c:axId val="92842754"/>
+        <c:axId val="51450963"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="16995230"/>
+        <c:axId val="92842754"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="90"/>
@@ -2014,7 +2078,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
+                  <a:rPr b="1" sz="900"/>
                   <a:t>age [years]</a:t>
                 </a:r>
               </a:p>
@@ -2032,12 +2096,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="18718344"/>
+        <c:crossAx val="51450963"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="20"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="18718344"/>
+        <c:axId val="51450963"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2053,7 +2117,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
+                  <a:rPr b="1" sz="900"/>
                   <a:t>Ainopyrine breath test [%dose kg mmol/CO2]</a:t>
                 </a:r>
               </a:p>
@@ -2071,8 +2135,8 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="16995230"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="92842754"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2101,15 +2165,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>213840</xdr:colOff>
+      <xdr:colOff>178200</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>141840</xdr:rowOff>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>818640</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>30960</xdr:rowOff>
+      <xdr:colOff>782280</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>146520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2124,8 +2188,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8021160" y="5934600"/>
-          <a:ext cx="4668480" cy="3515760"/>
+          <a:off x="8048160" y="5925600"/>
+          <a:ext cx="4668120" cy="3515400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2140,15 +2204,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>314640</xdr:colOff>
+      <xdr:colOff>279000</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>127080</xdr:rowOff>
+      <xdr:rowOff>89640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>831600</xdr:colOff>
+      <xdr:colOff>795240</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>115920</xdr:rowOff>
+      <xdr:rowOff>78120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2163,8 +2227,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8121960" y="9546480"/>
-          <a:ext cx="4580640" cy="3677040"/>
+          <a:off x="8148960" y="9537480"/>
+          <a:ext cx="4580280" cy="3676680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2179,15 +2243,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>248040</xdr:colOff>
+      <xdr:colOff>212400</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>676440</xdr:colOff>
+      <xdr:colOff>640080</xdr:colOff>
       <xdr:row>97</xdr:row>
-      <xdr:rowOff>43200</xdr:rowOff>
+      <xdr:rowOff>5400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2202,8 +2266,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8055360" y="13355280"/>
-          <a:ext cx="4492080" cy="3944520"/>
+          <a:off x="8082360" y="13346280"/>
+          <a:ext cx="4491720" cy="3944160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2218,15 +2282,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>576000</xdr:colOff>
+      <xdr:colOff>540000</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>152640</xdr:rowOff>
+      <xdr:rowOff>143640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>320760</xdr:colOff>
+      <xdr:colOff>284400</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>117360</xdr:rowOff>
+      <xdr:rowOff>79560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2241,8 +2305,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17132760" y="3508920"/>
-          <a:ext cx="8390880" cy="4337640"/>
+          <a:off x="17159760" y="3499920"/>
+          <a:ext cx="8390520" cy="4337280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2257,15 +2321,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>675720</xdr:colOff>
+      <xdr:colOff>639720</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>51120</xdr:rowOff>
+      <xdr:rowOff>13320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>273240</xdr:colOff>
+      <xdr:colOff>236880</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:rowOff>94680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2280,8 +2344,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17232480" y="7933680"/>
-          <a:ext cx="8243640" cy="4077000"/>
+          <a:off x="17259480" y="7924680"/>
+          <a:ext cx="8243280" cy="4076640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2296,15 +2360,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>703080</xdr:colOff>
+      <xdr:colOff>667080</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>40680</xdr:rowOff>
+      <xdr:rowOff>3240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>266040</xdr:colOff>
+      <xdr:colOff>229680</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>105120</xdr:rowOff>
+      <xdr:rowOff>66960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2319,8 +2383,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17259840" y="12072600"/>
-          <a:ext cx="7396200" cy="2522880"/>
+          <a:off x="17286840" y="12063600"/>
+          <a:ext cx="7395840" cy="2522520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2335,15 +2399,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>835920</xdr:colOff>
+      <xdr:colOff>863280</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>48960</xdr:rowOff>
+      <xdr:rowOff>39960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>441720</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>69840</xdr:rowOff>
+      <xdr:colOff>468360</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>97560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2351,8 +2415,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12706920" y="5534640"/>
-        <a:ext cx="4291560" cy="3186360"/>
+        <a:off x="12797280" y="5525640"/>
+        <a:ext cx="4290840" cy="3097800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2365,15 +2429,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>888120</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:colOff>915480</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>115200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>676800</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>71640</xdr:rowOff>
+      <xdr:colOff>703440</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>99360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2381,8 +2445,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12759120" y="9353160"/>
-        <a:ext cx="4474440" cy="3057480"/>
+        <a:off x="12849480" y="9255960"/>
+        <a:ext cx="4473720" cy="3057480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2395,15 +2459,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>834480</xdr:colOff>
+      <xdr:colOff>861840</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>140400</xdr:rowOff>
+      <xdr:rowOff>14760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>519120</xdr:colOff>
-      <xdr:row>89</xdr:row>
-      <xdr:rowOff>47160</xdr:rowOff>
+      <xdr:colOff>545760</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2411,8 +2475,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12705480" y="13094280"/>
-        <a:ext cx="4370400" cy="2980080"/>
+        <a:off x="12795840" y="12997080"/>
+        <a:ext cx="4369680" cy="2979720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2432,14 +2496,15 @@
   </sheetPr>
   <dimension ref="A1:Y130"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
-      <selection activeCell="G29" activeCellId="0" pane="topLeft" sqref="G29"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
+      <selection activeCell="C30" activeCellId="0" pane="topLeft" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7448979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4081632653061"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5969387755102"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7040816326531"/>
     <col collapsed="false" hidden="false" max="13" min="6" style="0" width="11.5204081632653"/>
@@ -3633,8 +3698,6 @@
         <v>0.485</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="20">
       <c r="A20" s="2" t="s">
         <v>60</v>
@@ -3905,8 +3968,6 @@
         <v>0.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="28">
       <c r="A28" s="2" t="s">
         <v>92</v>
@@ -3938,12 +3999,12 @@
         <v>96</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="30">
       <c r="A30" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>32</v>

</xml_diff>